<commit_message>
ng: add ONCHO pre stop form
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Nigeria/2023/ng_oncho_202301_prestop_2_participant.xlsx
+++ b/ONCHO/Impact Assessments/Nigeria/2023/ng_oncho_202301_prestop_2_participant.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -258,10 +258,10 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>(Aug 2022) ONCHO PreStop - 2. Participant Form</t>
-  </si>
-  <si>
-    <t>ng_oncho_prestop_2_participant_202208</t>
+    <t>(Jan 2023) ONCHO PreStop - 2. Participant Form</t>
+  </si>
+  <si>
+    <t>ng_oncho_202301_prestop_2_participant</t>
   </si>
   <si>
     <t>English</t>
@@ -274,8 +274,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -317,6 +317,134 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -325,134 +453,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -475,55 +475,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -535,127 +649,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -714,21 +714,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -740,24 +725,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -779,20 +751,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -811,148 +787,172 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1320,7 +1320,7 @@
   <sheetPr/>
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -2122,8 +2122,8 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>

</xml_diff>